<commit_message>
Create data and figures with strict term count as cut-off
</commit_message>
<xml_diff>
--- a/Mads/Resources/ElectronMicroscopyCollection/TopicsDataframe_Reduced.xlsx
+++ b/Mads/Resources/ElectronMicroscopyCollection/TopicsDataframe_Reduced.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +471,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Topic</t>
+          <t>Structural biology</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>topic_0003</t>
+          <t>topic_1317</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -488,30 +488,30 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Topic (0)</t>
+          <t>Structural biology (2)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Topic</t>
+          <t>Structural biology</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>topic_0003</t>
+          <t>topic_1317</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -519,30 +519,30 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Topic (0)</t>
+          <t>Structural biology (2)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Laboratory techniques</t>
+          <t>Electron microscopy</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>topic_3361</t>
+          <t>topic_0611</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -550,288 +550,40 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Laboratory techniques (1)</t>
+          <t>Electron microscopy (3)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Electron microscopy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>topic_3070</t>
+          <t>topic_0611</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Strict</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>Biology (1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Laboratory techniques</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>topic_3361</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>15</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Laboratory techniques (1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Biology</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>topic_3070</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>15</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Biology (1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Imaging</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>topic_3382</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Strict</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Imaging (2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Structural biology</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>topic_1317</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Strict</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>11</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Structural biology (2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Imaging</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>topic_3382</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>15</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Imaging (2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Structural biology</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>topic_1317</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Structural biology (2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Electron microscopy</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>topic_0611</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>3</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Strict</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>13</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Electron microscopy (3)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Electron microscopy</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>topic_0611</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>13</v>
-      </c>
-      <c r="G13" t="inlineStr">
         <is>
           <t>Electron microscopy (3)</t>
         </is>

</xml_diff>